<commit_message>
Feedback graph changed, open links after when break is going on,
changed the radar graph so that it does not show 0 in any field.
changed logic of event.js to suit the need of link opening before the break ends.
</commit_message>
<xml_diff>
--- a/Horarium Pricing.xlsx
+++ b/Horarium Pricing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Somewhere\Horarium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA9DCD5-5139-42CC-BE86-989E9557F16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88468EBE-A027-49A3-9107-87C439A868ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Dev</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>Total for us</t>
+  </si>
+  <si>
+    <t>Subscription</t>
+  </si>
+  <si>
+    <t>Per Year</t>
+  </si>
+  <si>
+    <t>expances</t>
+  </si>
+  <si>
+    <t>Excluding expances</t>
+  </si>
+  <si>
+    <t>Excluding costs</t>
   </si>
 </sst>
 </file>
@@ -462,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,10 +820,7 @@
         <v>5988.6</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E19" s="2" t="s">
         <v>22</v>
       </c>
@@ -840,10 +852,118 @@
         <v>8544.5999999999985</v>
       </c>
     </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="28" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A29" s="5"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="5"/>
+      <c r="G29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="C30" s="5">
+        <f>$G$30*B30</f>
+        <v>10500</v>
+      </c>
+      <c r="D30">
+        <f>$I$30*B30</f>
+        <v>8925</v>
+      </c>
+      <c r="G30">
+        <v>30000</v>
+      </c>
+      <c r="H30">
+        <v>4500</v>
+      </c>
+      <c r="I30">
+        <f>G30-H30</f>
+        <v>25500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="C31" s="5">
+        <f>$G$30*B31</f>
+        <v>12000</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:D32" si="0">$I$30*B31</f>
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="C32" s="5">
+        <f>$G$30*B32</f>
+        <v>7500</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>6375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A34" s="3"/>
+      <c r="B34" s="8">
+        <f>SUM(B29:B32)</f>
+        <v>1</v>
+      </c>
+      <c r="C34" s="6">
+        <f>SUM(C30:C32)</f>
+        <v>30000</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>